<commit_message>
Review file .mpp, CM
</commit_message>
<xml_diff>
--- a/Document/MonitorTracking/ReportMark.xlsx
+++ b/Document/MonitorTracking/ReportMark.xlsx
@@ -16,8 +16,60 @@
 </workbook>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="E6">
+      <text>
+        <r>
+          <rPr>
+            <rFont val="Calibri"/>
+            <charset val="1"/>
+            <family val="2"/>
+            <color rgb="00000000"/>
+            <sz val="11"/>
+          </rPr>
+          <t xml:space="preserve">Have good question to make clear issue about Portlet 1.0, 2.0</t>
+        </r>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F7">
+      <text>
+        <r>
+          <rPr>
+            <rFont val="Calibri"/>
+            <charset val="1"/>
+            <family val="2"/>
+            <color rgb="00000000"/>
+            <sz val="11"/>
+          </rPr>
+          <t xml:space="preserve">-2: Commit unneccessary folder into SVN “http://oopms.googlecode.com/svn/trunk/SourceCode/RequirementModule/build”</t>
+        </r>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F9">
+      <text>
+        <r>
+          <rPr>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <color rgb="00000000"/>
+            <sz val="11"/>
+          </rPr>
+          <t xml:space="preserve">-2: Commit unneccessary folder into SVN “http://oopms.googlecode.com/svn/trunk/SourceCode/PlannerModule/build
+-3: File .mpp has not updated</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="51">
   <si>
     <t>Document</t>
   </si>
@@ -133,6 +185,9 @@
     <t>17/7</t>
   </si>
   <si>
+    <t>18/7</t>
+  </si>
+  <si>
     <t>Duy</t>
   </si>
   <si>
@@ -151,7 +206,22 @@
     <t>Hai</t>
   </si>
   <si>
+    <t>Note:</t>
+  </si>
+  <si>
     <t>No update plan weekly</t>
+  </si>
+  <si>
+    <t>Minus: File .mpp has not updated</t>
+  </si>
+  <si>
+    <t>Pending issues:</t>
+  </si>
+  <si>
+    <t>Commit unneccessary into the SVN such as folder “build” within Project</t>
+  </si>
+  <si>
+    <t>The file .mpp has not updated % Completion of tasks</t>
   </si>
 </sst>
 </file>
@@ -161,7 +231,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -209,6 +279,19 @@
       <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
+      <color rgb="00000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="00FF0000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
       <color rgb="00000000"/>
       <sz val="11"/>
     </font>
@@ -325,7 +408,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="5" numFmtId="164" xfId="0">
@@ -388,15 +471,20 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="6" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="6" fontId="7" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="6" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="6" fontId="8" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="7" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="7" fontId="7" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="7" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="7" fontId="8" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="8" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="8" fontId="7" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="8" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="8" fontId="8" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -481,17 +569,17 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.2823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.3490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.79607843137255"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.0823529411765"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.66666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4549019607843"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.66666666666667"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.6117647058823"/>
-    <col collapsed="false" hidden="false" max="18" min="10" style="1" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.5176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.5137254901961"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.82745098039216"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.2039215686275"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.70196078431373"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.556862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.70196078431373"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.7686274509804"/>
+    <col collapsed="false" hidden="false" max="18" min="10" style="1" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.67843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="22.4" outlineLevel="0" r="1" s="3">
@@ -1737,17 +1825,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D14" activeCellId="0" pane="topLeft" sqref="D14"/>
+      <selection activeCell="A14" activeCellId="0" pane="topLeft" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.63921568627451"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.4823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5294117647059"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.1058823529412"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.67843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -1771,7 +1859,9 @@
       <c r="E3" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="24"/>
+      <c r="F3" s="24" t="s">
+        <v>38</v>
+      </c>
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
@@ -1783,17 +1873,17 @@
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4" s="28">
       <c r="A4" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="26" t="n">
         <v>100</v>
       </c>
       <c r="C4" s="27" t="n">
         <f aca="false">B4+SUM(E4:AA4)-SUM(E5:AA5)</f>
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E4" s="26"/>
       <c r="F4" s="26"/>
@@ -1811,164 +1901,196 @@
       <c r="B5" s="26"/>
       <c r="C5" s="27"/>
       <c r="D5" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="29" t="n">
+        <v>10</v>
+      </c>
+      <c r="F5" s="29" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6" s="32">
+      <c r="A6" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="30" t="n">
+        <v>100</v>
+      </c>
+      <c r="C6" s="31" t="n">
+        <f aca="false">B6+SUM(E6:AA6)-SUM(E7:AA7)</f>
+        <v>92</v>
+      </c>
+      <c r="D6" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="26" t="n">
-        <v>10</v>
-      </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6" s="31">
-      <c r="A6" s="29" t="s">
+      <c r="E6" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="7" s="32">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="29" t="n">
+      <c r="E7" s="33" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" s="30" t="n">
+        <f aca="false">3+2</f>
+        <v>5</v>
+      </c>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="8" s="36">
+      <c r="A8" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="34" t="n">
         <v>100</v>
       </c>
-      <c r="C6" s="30" t="n">
-        <f aca="false">B6+SUM(E6:AA6)-SUM(E7:AA7)</f>
-        <v>95</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="7" s="31">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="29" t="s">
+      <c r="C8" s="35" t="n">
+        <f aca="false">B8+SUM(E8:AA8)-SUM(E9:AA9)</f>
+        <v>90</v>
+      </c>
+      <c r="D8" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="29" t="n">
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="9" s="36">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="37" t="n">
         <v>5</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="8" s="34">
-      <c r="A8" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="32" t="n">
+      <c r="F9" s="37" t="n">
+        <f aca="false">3+2</f>
+        <v>5</v>
+      </c>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="10" s="32">
+      <c r="A10" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="30" t="n">
         <v>100</v>
       </c>
-      <c r="C8" s="33" t="n">
-        <f aca="false">B8+SUM(E8:AA8)-SUM(E9:AA9)</f>
-        <v>95</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="9" s="34">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="32" t="s">
+      <c r="C10" s="31" t="n">
+        <f aca="false">B10+SUM(E10:AA10)-SUM(E11:AA11)</f>
+        <v>92</v>
+      </c>
+      <c r="D10" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="32" t="n">
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="11" s="32">
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="33" t="n">
         <v>5</v>
       </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="10" s="31">
-      <c r="A10" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="29" t="n">
-        <v>100</v>
-      </c>
-      <c r="C10" s="30" t="n">
-        <f aca="false">B10+SUM(E10:AA10)-SUM(E11:AA11)</f>
-        <v>95</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="11" s="31">
-      <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="29" t="n">
-        <v>5</v>
-      </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
+      <c r="F11" s="33" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="13">
-      <c r="D13" s="0" t="s">
-        <v>6</v>
+      <c r="A13" s="38" t="s">
+        <v>45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="14">
-      <c r="E14" s="35" t="s">
-        <v>44</v>
+      <c r="E14" s="39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="15">
+      <c r="F15" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="17">
+      <c r="A17" s="38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="18">
+      <c r="B18" s="40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="19">
+      <c r="B19" s="40" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1979,6 +2101,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1994,7 +2117,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.67843137254902"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>